<commit_message>
add sleep mode and assertions
</commit_message>
<xml_diff>
--- a/docs/bill_of_materials.xlsx
+++ b/docs/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kok/CLionProjects/stm32f401-trash-module/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE7716F-1EDD-784F-98C8-27626D46DA25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E749F54-08D0-6742-B5A6-8E1570ABFC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7780" yWindow="3360" windowWidth="28040" windowHeight="17180" xr2:uid="{3925CBBA-9425-4243-AAD1-1C53B1364004}"/>
   </bookViews>
@@ -83,12 +83,6 @@
     <t>https://tpetrov.com/svetodiod-3mm-zelen-12mcd-246967</t>
   </si>
   <si>
-    <t>Resistor 300 Ohm</t>
-  </si>
-  <si>
-    <t>https://tpetrov.com/rezistor-330om-025w-14881</t>
-  </si>
-  <si>
     <t>https://tpetrov.com/kuplung-250-nx-03m-246741</t>
   </si>
   <si>
@@ -140,15 +134,9 @@
     <t>https://tpetrov.com/kondenzator-47mf-50v-smd-1206-245474</t>
   </si>
   <si>
-    <t>https://tpetrov.com/kondenzator-100nf-50v-250039</t>
-  </si>
-  <si>
     <t>R5…6</t>
   </si>
   <si>
-    <t>https://tpetrov.com/rezistor-10kom-06w-1-247145</t>
-  </si>
-  <si>
     <t>https://tpetrov.com/kuplung-250-nx-06m-241738</t>
   </si>
   <si>
@@ -164,9 +152,6 @@
     <t>C18</t>
   </si>
   <si>
-    <t>https://tpetrov.com/kondenzator-22mf-100v-105c-37954</t>
-  </si>
-  <si>
     <t>Connector M/F 01x02P2.50mm</t>
   </si>
   <si>
@@ -204,6 +189,21 @@
   </si>
   <si>
     <t>U3</t>
+  </si>
+  <si>
+    <t>https://tpetrov.com/rezistor-10kom-025w-smd-1206-239372</t>
+  </si>
+  <si>
+    <t>Resistor 330 Ohm</t>
+  </si>
+  <si>
+    <t>https://tpetrov.com/rezistor-330om-0125w-1-smd-243402</t>
+  </si>
+  <si>
+    <t>https://tpetrov.com/kondenzator-22uf-50v-smd-02-240100</t>
+  </si>
+  <si>
+    <t>https://tpetrov.com/kondenzator-100nf-25v-smd-0402-45886</t>
   </si>
 </sst>
 </file>
@@ -645,7 +645,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,10 +698,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
@@ -714,12 +714,12 @@
         <v>0.31</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -756,15 +756,15 @@
         <v>9.4600000000000009</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C6" s="4">
         <v>4</v>
@@ -777,12 +777,12 @@
         <v>0.24</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -798,12 +798,12 @@
         <v>0.16</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -819,12 +819,12 @@
         <v>0.12</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>10</v>
@@ -840,15 +840,15 @@
         <v>2.44</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -861,15 +861,15 @@
         <v>0.43</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -887,31 +887,31 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="4">
         <v>3</v>
       </c>
       <c r="D12" s="5">
-        <v>0.1</v>
+        <v>0.06</v>
       </c>
       <c r="E12" s="5">
         <f>C12*D12</f>
-        <v>0.30000000000000004</v>
+        <v>0.18</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C13" s="4">
         <v>2</v>
@@ -924,36 +924,36 @@
         <v>0.06</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
       </c>
       <c r="D14" s="5">
-        <v>0.13</v>
+        <v>0.08</v>
       </c>
       <c r="E14" s="5">
         <f>C14*D14</f>
-        <v>0.13</v>
+        <v>0.08</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C15" s="4">
         <v>2</v>
@@ -966,36 +966,36 @@
         <v>0.3</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="4">
         <v>4</v>
       </c>
       <c r="D16" s="5">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
       <c r="E16" s="5">
         <f>C16*D16</f>
-        <v>0.32</v>
+        <v>0.12</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
@@ -1008,15 +1008,15 @@
         <v>0.08</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
@@ -1029,12 +1029,12 @@
         <v>0.19</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>10</v>
@@ -1060,7 +1060,7 @@
       <c r="D20" s="9"/>
       <c r="E20" s="9">
         <f>SUM(E2:E19)</f>
-        <v>17.169999999999998</v>
+        <v>16.799999999999997</v>
       </c>
       <c r="F20" s="7"/>
     </row>
@@ -1068,17 +1068,14 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="F11" r:id="rId1" xr:uid="{90220F24-6D83-824C-92BA-1431B153E746}"/>
-    <hyperlink ref="F13" r:id="rId2" xr:uid="{9E900F7F-BB2E-4845-B105-5EFA6A97BD32}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{551C135B-CDCE-574D-8254-18A6AEA7A358}"/>
-    <hyperlink ref="F15" r:id="rId4" xr:uid="{23761C77-7ED4-6846-B681-6DEB6ACABC57}"/>
-    <hyperlink ref="F16" r:id="rId5" xr:uid="{03A9C16F-E0CB-AE4C-9614-5597E343752E}"/>
-    <hyperlink ref="F12" r:id="rId6" xr:uid="{A03C0725-487B-AB40-A0CA-412B1282F360}"/>
-    <hyperlink ref="F7" r:id="rId7" xr:uid="{0D7C8135-AAA1-544E-AB24-BC9768CA7DEC}"/>
-    <hyperlink ref="F8" r:id="rId8" xr:uid="{C72004BD-BF76-2E4B-BDD6-ADC9F774278A}"/>
-    <hyperlink ref="F14" r:id="rId9" xr:uid="{07681066-8E92-D741-8C2F-A3EFE0DE7287}"/>
-    <hyperlink ref="F6" r:id="rId10" xr:uid="{7A611CAD-499C-9148-B401-8A8E08534D81}"/>
-    <hyperlink ref="F17" r:id="rId11" xr:uid="{93C26B37-6E06-344C-A89C-EE8D38DCCE65}"/>
-    <hyperlink ref="F3" r:id="rId12" xr:uid="{62E4B2D0-2664-2A45-8CCC-855F07123A14}"/>
+    <hyperlink ref="F5" r:id="rId2" xr:uid="{551C135B-CDCE-574D-8254-18A6AEA7A358}"/>
+    <hyperlink ref="F15" r:id="rId3" xr:uid="{23761C77-7ED4-6846-B681-6DEB6ACABC57}"/>
+    <hyperlink ref="F7" r:id="rId4" xr:uid="{0D7C8135-AAA1-544E-AB24-BC9768CA7DEC}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{C72004BD-BF76-2E4B-BDD6-ADC9F774278A}"/>
+    <hyperlink ref="F6" r:id="rId6" xr:uid="{7A611CAD-499C-9148-B401-8A8E08534D81}"/>
+    <hyperlink ref="F17" r:id="rId7" xr:uid="{93C26B37-6E06-344C-A89C-EE8D38DCCE65}"/>
+    <hyperlink ref="F3" r:id="rId8" xr:uid="{62E4B2D0-2664-2A45-8CCC-855F07123A14}"/>
+    <hyperlink ref="F18" r:id="rId9" xr:uid="{24DC9FAA-ACA5-9B4F-86DE-E8FDCF38084E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
config gpios for low speed in order to reduce emi
</commit_message>
<xml_diff>
--- a/docs/bill_of_materials.xlsx
+++ b/docs/bill_of_materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kok/CLionProjects/stm32f401-trash-module/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E749F54-08D0-6742-B5A6-8E1570ABFC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4BAB74-F6EC-F84B-95F3-193EB33505F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="3360" windowWidth="28040" windowHeight="17180" xr2:uid="{3925CBBA-9425-4243-AAD1-1C53B1364004}"/>
+    <workbookView xWindow="1660" yWindow="1960" windowWidth="28040" windowHeight="17180" xr2:uid="{3925CBBA-9425-4243-AAD1-1C53B1364004}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -122,9 +122,6 @@
     <t>R2...4</t>
   </si>
   <si>
-    <t>C1,C3,C4,C5</t>
-  </si>
-  <si>
     <t>Capacitor 100 nF</t>
   </si>
   <si>
@@ -204,6 +201,9 @@
   </si>
   <si>
     <t>https://tpetrov.com/kondenzator-100nf-25v-smd-0402-45886</t>
+  </si>
+  <si>
+    <t>C1,C3,C4,C5, C7, C8</t>
   </si>
 </sst>
 </file>
@@ -645,13 +645,13 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -698,10 +698,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
@@ -714,12 +714,12 @@
         <v>0.31</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -761,10 +761,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" s="4">
         <v>4</v>
@@ -777,12 +777,12 @@
         <v>0.24</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>12</v>
@@ -798,12 +798,12 @@
         <v>0.16</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -903,15 +903,15 @@
         <v>0.18</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="4">
         <v>2</v>
@@ -924,15 +924,15 @@
         <v>0.06</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
@@ -945,15 +945,15 @@
         <v>0.08</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C15" s="4">
         <v>2</v>
@@ -966,15 +966,15 @@
         <v>0.3</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="C16" s="4">
         <v>4</v>
@@ -987,15 +987,15 @@
         <v>0.12</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
@@ -1008,7 +1008,7 @@
         <v>0.08</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1029,12 +1029,12 @@
         <v>0.19</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>10</v>
@@ -1076,6 +1076,7 @@
     <hyperlink ref="F17" r:id="rId7" xr:uid="{93C26B37-6E06-344C-A89C-EE8D38DCCE65}"/>
     <hyperlink ref="F3" r:id="rId8" xr:uid="{62E4B2D0-2664-2A45-8CCC-855F07123A14}"/>
     <hyperlink ref="F18" r:id="rId9" xr:uid="{24DC9FAA-ACA5-9B4F-86DE-E8FDCF38084E}"/>
+    <hyperlink ref="F16" r:id="rId10" xr:uid="{A74E18EF-6F86-DD47-ABB6-3642F7CD156E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor code and file structure
</commit_message>
<xml_diff>
--- a/docs/bill_of_materials.xlsx
+++ b/docs/bill_of_materials.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10118"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kok/CLionProjects/stm32f401-trash-module/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB4BAB74-F6EC-F84B-95F3-193EB33505F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8DC473-71F1-624F-B62F-A6E819E5B279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="1960" windowWidth="28040" windowHeight="17180" xr2:uid="{3925CBBA-9425-4243-AAD1-1C53B1364004}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Part</t>
   </si>
@@ -65,9 +65,6 @@
     <t>U2</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -204,6 +201,27 @@
   </si>
   <si>
     <t>C1,C3,C4,C5, C7, C8</t>
+  </si>
+  <si>
+    <t>J1, J5</t>
+  </si>
+  <si>
+    <t>Schottky Diode 1A</t>
+  </si>
+  <si>
+    <t>https://tpetrov.com/bat54j-sod323-40216</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>Polyfuse 300 mA</t>
+  </si>
+  <si>
+    <t>https://tpetrov.com/predpazitel-rxef030-244588</t>
+  </si>
+  <si>
+    <t>F1</t>
   </si>
 </sst>
 </file>
@@ -642,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34F765-CC6B-A549-B659-CF658C4B9F27}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,7 +687,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>4</v>
@@ -698,10 +716,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
@@ -714,12 +732,12 @@
         <v>0.31</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>8</v>
@@ -731,19 +749,19 @@
         <v>0</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ref="E4:E19" si="0">D4*C4</f>
+        <f t="shared" ref="E4:E21" si="0">D4*C4</f>
         <v>0</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -756,15 +774,15 @@
         <v>9.4600000000000009</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C6" s="4">
         <v>4</v>
@@ -777,15 +795,15 @@
         <v>0.24</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="4">
         <v>2</v>
@@ -798,36 +816,36 @@
         <v>0.16</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="C8" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D8" s="5">
         <v>0.06</v>
       </c>
       <c r="E8" s="5">
         <f>C8*D8</f>
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -840,15 +858,15 @@
         <v>2.44</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
@@ -861,15 +879,15 @@
         <v>0.43</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -882,15 +900,15 @@
         <v>0.15</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="C12" s="4">
         <v>3</v>
@@ -903,15 +921,15 @@
         <v>0.18</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="4">
         <v>2</v>
@@ -924,15 +942,15 @@
         <v>0.06</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
@@ -945,15 +963,15 @@
         <v>0.08</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="4">
         <v>2</v>
@@ -966,15 +984,15 @@
         <v>0.3</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C16" s="4">
         <v>4</v>
@@ -987,15 +1005,15 @@
         <v>0.12</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
@@ -1008,15 +1026,15 @@
         <v>0.08</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="C18" s="4">
         <v>1</v>
@@ -1029,40 +1047,82 @@
         <v>0.19</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C19" s="4">
         <v>1</v>
       </c>
       <c r="D19" s="5">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="E19" s="5">
         <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0.61</v>
+      </c>
+      <c r="E20" s="5">
+        <f>C20*D20</f>
+        <v>0.61</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5">
         <v>0</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9">
-        <f>SUM(E2:E19)</f>
-        <v>16.799999999999997</v>
-      </c>
-      <c r="F20" s="7"/>
+      <c r="E21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9">
+        <f>SUM(E2:E21)</f>
+        <v>17.679999999999996</v>
+      </c>
+      <c r="F22" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
refactor ISR's to have minimal code
</commit_message>
<xml_diff>
--- a/docs/bill_of_materials.xlsx
+++ b/docs/bill_of_materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kok/CLionProjects/stm32f401-trash-module/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EF6209E-4D8A-6F43-B04C-834285761500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D95CAD-0DDD-DF43-82D3-819E970D750B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1660" yWindow="1960" windowWidth="28040" windowHeight="17180" xr2:uid="{3925CBBA-9425-4243-AAD1-1C53B1364004}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="65">
   <si>
     <t>Part</t>
   </si>
@@ -203,9 +203,6 @@
     <t>C1,C3,C4,C5, C7, C8</t>
   </si>
   <si>
-    <t>J1, J5</t>
-  </si>
-  <si>
     <t>Schottky Diode 1A</t>
   </si>
   <si>
@@ -222,6 +219,18 @@
   </si>
   <si>
     <t>F1</t>
+  </si>
+  <si>
+    <t>Connector M/F 01X04P2.50mm</t>
+  </si>
+  <si>
+    <t>https://tpetrov.com/kuplung-250-nx-04m-40813</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J5</t>
   </si>
 </sst>
 </file>
@@ -660,10 +669,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D34F765-CC6B-A549-B659-CF658C4B9F27}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,7 +758,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" ref="E4:E21" si="0">D4*C4</f>
+        <f t="shared" ref="E4:E22" si="0">D4*C4</f>
         <v>0</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -824,17 +833,17 @@
         <v>33</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C8" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D8" s="5">
         <v>0.06</v>
       </c>
       <c r="E8" s="5">
         <f>C8*D8</f>
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>14</v>
@@ -842,303 +851,325 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="E9" s="5">
+        <f>C9*D9</f>
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="5">
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5">
         <v>2.44</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E10" s="5">
         <f t="shared" si="0"/>
         <v>2.44</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5">
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
         <v>0.43</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E11" s="5">
         <f t="shared" si="0"/>
         <v>0.43</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F11" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5">
         <v>0.15</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E12" s="5">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F12" s="6" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" s="4">
-        <v>3</v>
-      </c>
-      <c r="D12" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="E12" s="5">
-        <f>C12*D12</f>
-        <v>0.18</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="4">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.06</v>
+      </c>
+      <c r="E13" s="5">
+        <f>C13*D13</f>
+        <v>0.18</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C14" s="4">
         <v>2</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D14" s="5">
         <v>0.03</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E14" s="5">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="F14" s="6" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1</v>
-      </c>
-      <c r="D14" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="E14" s="5">
-        <f>C14*D14</f>
-        <v>0.08</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C15" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" s="5">
-        <v>0.15</v>
+        <v>0.08</v>
       </c>
       <c r="E15" s="5">
         <f>C15*D15</f>
-        <v>0.3</v>
+        <v>0.08</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C16" s="4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D16" s="5">
-        <v>0.03</v>
+        <v>0.15</v>
       </c>
       <c r="E16" s="5">
         <f>C16*D16</f>
-        <v>0.12</v>
+        <v>0.3</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="C17" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D17" s="5">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
       <c r="E17" s="5">
         <f>C17*D17</f>
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.08</v>
+      </c>
+      <c r="E18" s="5">
+        <f>C18*D18</f>
+        <v>0.08</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="4">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5">
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
         <v>0.19</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E19" s="5">
         <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F19" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C19" s="4">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="4">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
         <v>0.15</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E20" s="5">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="4">
-        <v>1</v>
-      </c>
-      <c r="D20" s="5">
-        <v>0.61</v>
-      </c>
-      <c r="E20" s="5">
-        <f>C20*D20</f>
-        <v>0.61</v>
-      </c>
       <c r="F20" s="6" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.61</v>
+      </c>
+      <c r="E21" s="5">
+        <f>C21*D21</f>
+        <v>0.61</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="4">
-        <v>1</v>
-      </c>
-      <c r="D21" s="5">
+      <c r="C22" s="4">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5">
         <v>0</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E22" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F21" s="6" t="s">
+      <c r="F22" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9">
-        <f>SUM(E2:E21)</f>
-        <v>17.679999999999996</v>
-      </c>
-      <c r="F22" s="7"/>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9">
+        <f>SUM(E2:E22)</f>
+        <v>17.759999999999994</v>
+      </c>
+      <c r="F23" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F11" r:id="rId1" xr:uid="{90220F24-6D83-824C-92BA-1431B153E746}"/>
+    <hyperlink ref="F12" r:id="rId1" xr:uid="{90220F24-6D83-824C-92BA-1431B153E746}"/>
     <hyperlink ref="F5" r:id="rId2" xr:uid="{551C135B-CDCE-574D-8254-18A6AEA7A358}"/>
-    <hyperlink ref="F15" r:id="rId3" xr:uid="{23761C77-7ED4-6846-B681-6DEB6ACABC57}"/>
+    <hyperlink ref="F16" r:id="rId3" xr:uid="{23761C77-7ED4-6846-B681-6DEB6ACABC57}"/>
     <hyperlink ref="F7" r:id="rId4" xr:uid="{0D7C8135-AAA1-544E-AB24-BC9768CA7DEC}"/>
     <hyperlink ref="F8" r:id="rId5" xr:uid="{C72004BD-BF76-2E4B-BDD6-ADC9F774278A}"/>
     <hyperlink ref="F6" r:id="rId6" xr:uid="{7A611CAD-499C-9148-B401-8A8E08534D81}"/>
-    <hyperlink ref="F17" r:id="rId7" xr:uid="{93C26B37-6E06-344C-A89C-EE8D38DCCE65}"/>
+    <hyperlink ref="F18" r:id="rId7" xr:uid="{93C26B37-6E06-344C-A89C-EE8D38DCCE65}"/>
     <hyperlink ref="F3" r:id="rId8" xr:uid="{62E4B2D0-2664-2A45-8CCC-855F07123A14}"/>
-    <hyperlink ref="F18" r:id="rId9" xr:uid="{24DC9FAA-ACA5-9B4F-86DE-E8FDCF38084E}"/>
-    <hyperlink ref="F16" r:id="rId10" xr:uid="{A74E18EF-6F86-DD47-ABB6-3642F7CD156E}"/>
-    <hyperlink ref="F19" r:id="rId11" xr:uid="{BD10BCB3-E1B8-9A4C-8334-7BC634AC58E3}"/>
-    <hyperlink ref="F20" r:id="rId12" xr:uid="{49CC3ECD-B8D4-5B48-9D51-CB55D8DAA1D8}"/>
+    <hyperlink ref="F19" r:id="rId9" xr:uid="{24DC9FAA-ACA5-9B4F-86DE-E8FDCF38084E}"/>
+    <hyperlink ref="F17" r:id="rId10" xr:uid="{A74E18EF-6F86-DD47-ABB6-3642F7CD156E}"/>
+    <hyperlink ref="F20" r:id="rId11" xr:uid="{BD10BCB3-E1B8-9A4C-8334-7BC634AC58E3}"/>
+    <hyperlink ref="F21" r:id="rId12" xr:uid="{49CC3ECD-B8D4-5B48-9D51-CB55D8DAA1D8}"/>
+    <hyperlink ref="F9" r:id="rId13" xr:uid="{62BB0E09-C9BA-904D-B6F1-2838205F7B07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>